<commit_message>
Revert "update template file"
This reverts commit ce3557d1df6f5a77de36d6c544f19379343c1a00.
</commit_message>
<xml_diff>
--- a/addons/fleet_trip/static/src/template/MY_TEMPLATE.xlsx
+++ b/addons/fleet_trip/static/src/template/MY_TEMPLATE.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Documents\quanlyvantai-main\vantai-gateway-main\addons\fleet_trip\static\src\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\GitHub\vantai-gateway\addons\fleet_trip\static\src\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F193BF-F8BE-4FB3-AF63-A93336B9B908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="843"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="843" xr2:uid="{AE80BFCB-E5C5-467A-BBF7-7BAB7D7FE7A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="10" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" refMode="R1C1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,12 +33,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>HVKHQS</author>
   </authors>
   <commentList>
-    <comment ref="A3" authorId="0" shapeId="0">
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{C88B0D85-43D9-4A41-A26B-D04AEB241F76}">
       <text>
         <r>
           <rPr>
@@ -51,7 +52,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A4" authorId="0" shapeId="0">
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{A10E06F8-567E-424F-87D4-02852CE99145}">
       <text>
         <r>
           <rPr>
@@ -65,7 +66,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E4" authorId="0" shapeId="0">
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{75B6EC33-5246-45A1-811A-0C731BCE16AE}">
       <text>
         <r>
           <rPr>
@@ -79,7 +80,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F9" authorId="0" shapeId="0">
+    <comment ref="F9" authorId="0" shapeId="0" xr:uid="{5B6EADB5-F96A-43AD-BFEC-3EA8E232E834}">
       <text>
         <r>
           <rPr>
@@ -93,7 +94,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F20" authorId="0" shapeId="0">
+    <comment ref="F20" authorId="0" shapeId="0" xr:uid="{10EBADF3-5482-4960-A93F-41C65AB27490}">
       <text>
         <r>
           <rPr>
@@ -107,7 +108,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A25" authorId="0" shapeId="0">
+    <comment ref="A25" authorId="0" shapeId="0" xr:uid="{9EC90B19-ACB5-43D4-ADBA-E8D9F1899988}">
       <text>
         <r>
           <rPr>
@@ -121,7 +122,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F25" authorId="0" shapeId="0">
+    <comment ref="F25" authorId="0" shapeId="0" xr:uid="{A91EB64E-61A0-4201-94A9-62BFD66311CF}">
       <text>
         <r>
           <rPr>
@@ -135,7 +136,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C27" authorId="0" shapeId="0">
+    <comment ref="C27" authorId="0" shapeId="0" xr:uid="{78436B62-7008-4FD7-81E9-B816EC1D8BED}">
       <text>
         <r>
           <rPr>
@@ -149,7 +150,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C32" authorId="0" shapeId="0">
+    <comment ref="C32" authorId="0" shapeId="0" xr:uid="{8A95AE7B-5998-433C-95CE-45BD538D95FB}">
       <text>
         <r>
           <rPr>
@@ -281,7 +282,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="22">
     <font>
       <sz val="10"/>
@@ -520,7 +521,7 @@
         <xdr:cNvPr id="10106" name="Line 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{749D7FC7-DFAD-C43D-9AF1-AB5E95A3655B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{749D7FC7-DFAD-C43D-9AF1-AB5E95A3655B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -574,7 +575,7 @@
         <xdr:cNvPr id="10107" name="Line 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E2163BCC-6786-BB74-767D-C44461EBDE69}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2163BCC-6786-BB74-767D-C44461EBDE69}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -870,12 +871,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D3FC8AD-A681-4BBB-A349-157E28EC377A}">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25:M25"/>
-    </sheetView>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
   <cols>
@@ -1324,16 +1323,16 @@
       <c r="C25" s="18"/>
       <c r="D25" s="18"/>
       <c r="E25" s="3"/>
-      <c r="F25" s="19" t="s">
+      <c r="F25" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="19"/>
-      <c r="K25" s="19"/>
-      <c r="L25" s="19"/>
-      <c r="M25" s="19"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
+      <c r="M25" s="18"/>
     </row>
     <row r="26" spans="1:13" s="9" customFormat="1" ht="15.75">
       <c r="A26" s="8"/>
@@ -1507,7 +1506,7 @@
       <c r="M36" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="12">
     <mergeCell ref="C27:K27"/>
     <mergeCell ref="C26:K26"/>
     <mergeCell ref="A20:D20"/>
@@ -1520,7 +1519,6 @@
     <mergeCell ref="E4:M4"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="E3:M3"/>
-    <mergeCell ref="F25:M25"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0" right="0" top="0.25" bottom="0" header="0.5" footer="0.5"/>

</xml_diff>